<commit_message>
uses dictionary to store column names in gen_data.py
</commit_message>
<xml_diff>
--- a/azfar/output.xlsx
+++ b/azfar/output.xlsx
@@ -577,7 +577,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>signup pages</t>
+          <t>Signup Pages</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
@@ -588,23 +588,23 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>barber qqqqqqq sdn bhd</t>
+          <t>Barber Qqqqqqq Sdn Bhd</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>unit b-07-3</t>
+          <t>Unit B-07-3</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
-          <t>kuala lumpur</t>
+          <t>Kuala Lumpur</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>kuala lumpur</t>
+          <t>Kuala Lumpur</t>
         </is>
       </c>
       <c r="J2" t="n">
@@ -633,7 +633,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>signup pages</t>
+          <t>Signup Pages</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -644,7 +644,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>barber qqqqqqq sdn bhd</t>
+          <t>Barber Qqqqqqq Sdn Bhd</t>
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
@@ -659,26 +659,26 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>ahmad</t>
+          <t>Ahmad</t>
         </is>
       </c>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr">
         <is>
-          <t>executive</t>
+          <t>Executive</t>
         </is>
       </c>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>b2c</t>
+          <t>B2C</t>
         </is>
       </c>
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr">
         <is>
-          <t>jnt</t>
+          <t>Jnt</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
@@ -688,7 +688,7 @@
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>service logistics</t>
+          <t>Service Logistics</t>
         </is>
       </c>
       <c r="V3" t="inlineStr"/>
@@ -703,7 +703,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>twitter</t>
+          <t>Twitter</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -714,27 +714,27 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>cakeeeeee central sdn bhd</t>
+          <t>Cakeeeeee Central Sdn Bhd</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>36 jalan pju 1a/12,</t>
+          <t>36 Jalan Pju 1A/12,</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>taman perindustrian jaya</t>
+          <t>Taman Perindustrian Jaya</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>petaling jaya</t>
+          <t>Petaling Jaya</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>kuala lumpur</t>
+          <t>Kuala Lumpur</t>
         </is>
       </c>
       <c r="J4" t="n">
@@ -763,7 +763,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>exhibition</t>
+          <t>Exhibition</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
@@ -774,27 +774,27 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>ddd automotive</t>
+          <t>Ddd Automotive</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>12 jalan astaka u8/l,</t>
+          <t>12 Jalan Astaka U8/L,</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>bukit jelutong</t>
+          <t>Bukit Jelutong</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>shah alam</t>
+          <t>Shah Alam</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>selangor</t>
+          <t>Selangor</t>
         </is>
       </c>
       <c r="J5" t="n">
@@ -803,13 +803,13 @@
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
-          <t>zhong</t>
+          <t>Zhong</t>
         </is>
       </c>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr">
         <is>
-          <t>director</t>
+          <t>Director</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -820,7 +820,7 @@
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>b2c</t>
+          <t>B2C</t>
         </is>
       </c>
       <c r="R5" t="inlineStr"/>
@@ -839,7 +839,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>facebook</t>
+          <t>Facebook</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -850,7 +850,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>fgfgff-line sdn bhd</t>
+          <t>Fgfgff-Line Sdn Bhd</t>
         </is>
       </c>
       <c r="F6" t="inlineStr"/>
@@ -861,7 +861,7 @@
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
-          <t>kula</t>
+          <t>Kula</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -871,7 +871,7 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>technician</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
@@ -882,7 +882,7 @@
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>b2c</t>
+          <t>B2C</t>
         </is>
       </c>
       <c r="R6" t="inlineStr"/>
@@ -894,7 +894,7 @@
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>chemical and energy</t>
+          <t>Chemical And Energy</t>
         </is>
       </c>
       <c r="V6" t="inlineStr"/>
@@ -911,7 +911,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>signup pages</t>
+          <t>Signup Pages</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
@@ -922,7 +922,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>perfect company</t>
+          <t>Perfect Company</t>
         </is>
       </c>
       <c r="F7" t="inlineStr"/>
@@ -960,27 +960,27 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>rrrworth sdn bhd</t>
+          <t>Rrrworth Sdn Bhd</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>lot f-1</t>
+          <t>Lot F-1</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> mpl saguking industrial estate. jalan</t>
+          <t xml:space="preserve"> Mpl Saguking Industrial Estate. Jalan</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>xx</t>
+          <t>Xx</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>selangor</t>
+          <t>Selangor</t>
         </is>
       </c>
       <c r="J8" t="n">
@@ -989,7 +989,7 @@
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
-          <t>adam</t>
+          <t>Adam</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -1002,7 +1002,7 @@
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>b2b</t>
+          <t>B2B</t>
         </is>
       </c>
       <c r="R8" t="inlineStr"/>
@@ -1021,7 +1021,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>exhibition</t>
+          <t>Exhibition</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
@@ -1032,7 +1032,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>tttt technologies sdn bhd</t>
+          <t>Tttt Technologies Sdn Bhd</t>
         </is>
       </c>
       <c r="F9" t="inlineStr"/>
@@ -1048,13 +1048,13 @@
       <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>b2b</t>
+          <t>B2B</t>
         </is>
       </c>
       <c r="R9" t="inlineStr"/>
       <c r="S9" t="inlineStr">
         <is>
-          <t>shopee express</t>
+          <t>Shopee Express</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
@@ -1064,7 +1064,7 @@
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>manufacturing</t>
+          <t>Manufacturing</t>
         </is>
       </c>
       <c r="V9" t="inlineStr"/>
@@ -1081,7 +1081,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>instagram</t>
+          <t>Instagram</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -1092,27 +1092,27 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>uuuutech logistic</t>
+          <t>Uuuutech Logistic</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>lot 77, pt 5118, no.5 (ground floor),</t>
+          <t>Lot 77, Pt 5118, No.5 (Ground Floor),</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>jalan prima 5,</t>
+          <t>Jalan Prima 5,</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>port dickson</t>
+          <t>Port Dickson</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>melaka</t>
+          <t>Melaka</t>
         </is>
       </c>
       <c r="J10" t="n">
@@ -1141,7 +1141,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>signup pages</t>
+          <t>Signup Pages</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
@@ -1152,27 +1152,27 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>uuuuu works sdn bhd</t>
+          <t>Uuuuu Works Sdn Bhd</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>28 jalan bs 9/10,</t>
+          <t>28 Jalan Bs 9/10,</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>kaw perindustrian bs 9</t>
+          <t>Kaw Perindustrian Bs 9</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>seri kembangan</t>
+          <t>Seri Kembangan</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>selangor</t>
+          <t>Selangor</t>
         </is>
       </c>
       <c r="J11" t="n">
@@ -1181,7 +1181,7 @@
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr">
         <is>
-          <t>far</t>
+          <t>Far</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
@@ -1191,7 +1191,7 @@
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>cleaner</t>
+          <t>Cleaner</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
@@ -1202,7 +1202,7 @@
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>b2b</t>
+          <t>B2B</t>
         </is>
       </c>
       <c r="R11" t="inlineStr"/>
@@ -1221,7 +1221,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>twitter</t>
+          <t>Twitter</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
@@ -1232,27 +1232,27 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>yyyyyy engineering and construction sdn bhd</t>
+          <t>Yyyyyy Engineering And Construction Sdn Bhd</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>no 20 jalan bakti</t>
+          <t>No 20 Jalan Bakti</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>65 taman mutiara rini skuda</t>
+          <t>65 Taman Mutiara Rini Skuda</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>xx</t>
+          <t>Xx</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>selangor</t>
+          <t>Selangor</t>
         </is>
       </c>
       <c r="J12" t="n">
@@ -1261,13 +1261,13 @@
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr">
         <is>
-          <t>wan</t>
+          <t>Wan</t>
         </is>
       </c>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr">
         <is>
-          <t>secretrary</t>
+          <t>Secretrary</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
@@ -1278,7 +1278,7 @@
       <c r="P12" t="inlineStr"/>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>b2c</t>
+          <t>B2C</t>
         </is>
       </c>
       <c r="R12" t="inlineStr"/>
@@ -1297,7 +1297,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>facebook</t>
+          <t>Facebook</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
@@ -1308,23 +1308,23 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>zzzzzzfab industries sdn bhd</t>
+          <t>Zzzzzzfab Industries Sdn Bhd</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>29, jalan meru indah 20,</t>
+          <t>29, Jalan Meru Indah 20,</t>
         </is>
       </c>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr">
         <is>
-          <t>klang</t>
+          <t>Klang</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>selangor</t>
+          <t>Selangor</t>
         </is>
       </c>
       <c r="J13" t="n">
@@ -1509,7 +1509,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>signup pages</t>
+          <t>Signup Pages</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
@@ -1520,27 +1520,27 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>uuuuu works sdn bhd</t>
+          <t>Uuuuu Works Sdn Bhd</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>28 jalan bs 9/10,</t>
+          <t>28 Jalan Bs 9/10,</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>kaw perindustrian bs 9</t>
+          <t>Kaw Perindustrian Bs 9</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>seri kembangan</t>
+          <t>Seri Kembangan</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>selangor</t>
+          <t>Selangor</t>
         </is>
       </c>
       <c r="J2" t="n">
@@ -1549,7 +1549,7 @@
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr">
         <is>
-          <t>far</t>
+          <t>Far</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -1559,7 +1559,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>cleaner</t>
+          <t>Cleaner</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -1570,7 +1570,7 @@
       <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>b2b</t>
+          <t>B2B</t>
         </is>
       </c>
       <c r="R2" t="inlineStr"/>
@@ -1590,7 +1590,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>exhibition</t>
+          <t>Exhibition</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -1601,27 +1601,27 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>ddd automotive</t>
+          <t>Ddd Automotive</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>12 jalan astaka u8/l,</t>
+          <t>12 Jalan Astaka U8/L,</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>bukit jelutong</t>
+          <t>Bukit Jelutong</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>shah alam</t>
+          <t>Shah Alam</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>selangor</t>
+          <t>Selangor</t>
         </is>
       </c>
       <c r="J3" t="n">
@@ -1630,13 +1630,13 @@
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
-          <t>zhong</t>
+          <t>Zhong</t>
         </is>
       </c>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr">
         <is>
-          <t>director</t>
+          <t>Director</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -1647,7 +1647,7 @@
       <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>b2c</t>
+          <t>B2C</t>
         </is>
       </c>
       <c r="R3" t="inlineStr"/>
@@ -1667,7 +1667,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>twitter</t>
+          <t>Twitter</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -1678,27 +1678,27 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>yyyyyy engineering and construction sdn bhd</t>
+          <t>Yyyyyy Engineering And Construction Sdn Bhd</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>no 20 jalan bakti</t>
+          <t>No 20 Jalan Bakti</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>65 taman mutiara rini skuda</t>
+          <t>65 Taman Mutiara Rini Skuda</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>xx</t>
+          <t>Xx</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>selangor</t>
+          <t>Selangor</t>
         </is>
       </c>
       <c r="J4" t="n">
@@ -1707,13 +1707,13 @@
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr">
         <is>
-          <t>wan</t>
+          <t>Wan</t>
         </is>
       </c>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr">
         <is>
-          <t>secretrary</t>
+          <t>Secretrary</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
@@ -1724,7 +1724,7 @@
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>b2c</t>
+          <t>B2C</t>
         </is>
       </c>
       <c r="R4" t="inlineStr"/>
@@ -1744,7 +1744,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>signup pages</t>
+          <t>Signup Pages</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
@@ -1755,23 +1755,23 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>barber qqqqqqq sdn bhd</t>
+          <t>Barber Qqqqqqq Sdn Bhd</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>unit b-07-3</t>
+          <t>Unit B-07-3</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
-          <t>kuala lumpur</t>
+          <t>Kuala Lumpur</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>kuala lumpur</t>
+          <t>Kuala Lumpur</t>
         </is>
       </c>
       <c r="J5" t="n">
@@ -1784,26 +1784,26 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>ahmad</t>
+          <t>Ahmad</t>
         </is>
       </c>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr">
         <is>
-          <t>executive</t>
+          <t>Executive</t>
         </is>
       </c>
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>b2c</t>
+          <t>B2C</t>
         </is>
       </c>
       <c r="R5" t="inlineStr"/>
       <c r="S5" t="inlineStr">
         <is>
-          <t>jnt</t>
+          <t>Jnt</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
@@ -1813,7 +1813,7 @@
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>service logistics</t>
+          <t>Service Logistics</t>
         </is>
       </c>
       <c r="V5" t="inlineStr"/>
@@ -1833,7 +1833,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>facebook</t>
+          <t>Facebook</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -1844,7 +1844,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>fgfgff-line sdn bhd</t>
+          <t>Fgfgff-Line Sdn Bhd</t>
         </is>
       </c>
       <c r="F6" t="inlineStr"/>
@@ -1855,7 +1855,7 @@
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
-          <t>kula</t>
+          <t>Kula</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -1865,7 +1865,7 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>technician</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
@@ -1876,7 +1876,7 @@
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>b2c</t>
+          <t>B2C</t>
         </is>
       </c>
       <c r="R6" t="inlineStr"/>
@@ -1888,7 +1888,7 @@
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>chemical and energy</t>
+          <t>Chemical And Energy</t>
         </is>
       </c>
       <c r="V6" t="inlineStr"/>
@@ -1913,27 +1913,27 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>rrrworth sdn bhd</t>
+          <t>Rrrworth Sdn Bhd</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>lot f-1</t>
+          <t>Lot F-1</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> mpl saguking industrial estate. jalan</t>
+          <t xml:space="preserve"> Mpl Saguking Industrial Estate. Jalan</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>xx</t>
+          <t>Xx</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>selangor</t>
+          <t>Selangor</t>
         </is>
       </c>
       <c r="J7" t="n">
@@ -1942,7 +1942,7 @@
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr">
         <is>
-          <t>adam</t>
+          <t>Adam</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -1955,7 +1955,7 @@
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>b2b</t>
+          <t>B2B</t>
         </is>
       </c>
       <c r="R7" t="inlineStr"/>
@@ -1975,7 +1975,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>twitter</t>
+          <t>Twitter</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -1986,27 +1986,27 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>cakeeeeee central sdn bhd</t>
+          <t>Cakeeeeee Central Sdn Bhd</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>36 jalan pju 1a/12,</t>
+          <t>36 Jalan Pju 1A/12,</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>taman perindustrian jaya</t>
+          <t>Taman Perindustrian Jaya</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>petaling jaya</t>
+          <t>Petaling Jaya</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>kuala lumpur</t>
+          <t>Kuala Lumpur</t>
         </is>
       </c>
       <c r="J8" t="n">
@@ -2036,7 +2036,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>exhibition</t>
+          <t>Exhibition</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
@@ -2047,7 +2047,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>tttt technologies sdn bhd</t>
+          <t>Tttt Technologies Sdn Bhd</t>
         </is>
       </c>
       <c r="F9" t="inlineStr"/>
@@ -2063,13 +2063,13 @@
       <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>b2b</t>
+          <t>B2B</t>
         </is>
       </c>
       <c r="R9" t="inlineStr"/>
       <c r="S9" t="inlineStr">
         <is>
-          <t>shopee express</t>
+          <t>Shopee Express</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
@@ -2079,7 +2079,7 @@
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>manufacturing</t>
+          <t>Manufacturing</t>
         </is>
       </c>
       <c r="V9" t="inlineStr"/>
@@ -2097,7 +2097,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>instagram</t>
+          <t>Instagram</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -2108,27 +2108,27 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>uuuutech logistic</t>
+          <t>Uuuutech Logistic</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>lot 77, pt 5118, no.5 (ground floor),</t>
+          <t>Lot 77, Pt 5118, No.5 (Ground Floor),</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>jalan prima 5,</t>
+          <t>Jalan Prima 5,</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>port dickson</t>
+          <t>Port Dickson</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>melaka</t>
+          <t>Melaka</t>
         </is>
       </c>
       <c r="J10" t="n">
@@ -2158,7 +2158,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>facebook</t>
+          <t>Facebook</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
@@ -2169,23 +2169,23 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>zzzzzzfab industries sdn bhd</t>
+          <t>Zzzzzzfab Industries Sdn Bhd</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>29, jalan meru indah 20,</t>
+          <t>29, Jalan Meru Indah 20,</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
-          <t>klang</t>
+          <t>Klang</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>selangor</t>
+          <t>Selangor</t>
         </is>
       </c>
       <c r="J11" t="n">
@@ -2215,7 +2215,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>signup pages</t>
+          <t>Signup Pages</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
@@ -2226,7 +2226,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>perfect company</t>
+          <t>Perfect Company</t>
         </is>
       </c>
       <c r="F12" t="inlineStr"/>
@@ -2339,27 +2339,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>uuuuu works sdn bhd</t>
+          <t>Uuuuu Works Sdn Bhd</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>28 jalan bs 9/10,</t>
+          <t>28 Jalan Bs 9/10,</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>kaw perindustrian bs 9</t>
+          <t>Kaw Perindustrian Bs 9</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>seri kembangan</t>
+          <t>Seri Kembangan</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>selangor</t>
+          <t>Selangor</t>
         </is>
       </c>
       <c r="G2" t="n">
@@ -2368,7 +2368,7 @@
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>b2b</t>
+          <t>B2B</t>
         </is>
       </c>
       <c r="J2" t="inlineStr"/>
@@ -2381,27 +2381,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ddd automotive</t>
+          <t>Ddd Automotive</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>12 jalan astaka u8/l,</t>
+          <t>12 Jalan Astaka U8/L,</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>bukit jelutong</t>
+          <t>Bukit Jelutong</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>shah alam</t>
+          <t>Shah Alam</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>selangor</t>
+          <t>Selangor</t>
         </is>
       </c>
       <c r="G3" t="n">
@@ -2410,7 +2410,7 @@
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
-          <t>b2c</t>
+          <t>B2C</t>
         </is>
       </c>
       <c r="J3" t="inlineStr"/>
@@ -2423,27 +2423,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>yyyyyy engineering and construction sdn bhd</t>
+          <t>Yyyyyy Engineering And Construction Sdn Bhd</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>no 20 jalan bakti</t>
+          <t>No 20 Jalan Bakti</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>65 taman mutiara rini skuda</t>
+          <t>65 Taman Mutiara Rini Skuda</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>xx</t>
+          <t>Xx</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>selangor</t>
+          <t>Selangor</t>
         </is>
       </c>
       <c r="G4" t="n">
@@ -2452,7 +2452,7 @@
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
         <is>
-          <t>b2c</t>
+          <t>B2C</t>
         </is>
       </c>
       <c r="J4" t="inlineStr"/>
@@ -2465,23 +2465,23 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>barber qqqqqqq sdn bhd</t>
+          <t>Barber Qqqqqqq Sdn Bhd</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>unit b-07-3</t>
+          <t>Unit B-07-3</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
-          <t>kuala lumpur</t>
+          <t>Kuala Lumpur</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>kuala lumpur</t>
+          <t>Kuala Lumpur</t>
         </is>
       </c>
       <c r="G5" t="n">
@@ -2489,12 +2489,12 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>service logistics</t>
+          <t>Service Logistics</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>b2c</t>
+          <t>B2C</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -2511,7 +2511,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>fgfgff-line sdn bhd</t>
+          <t>Fgfgff-Line Sdn Bhd</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -2521,12 +2521,12 @@
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
-          <t>chemical and energy</t>
+          <t>Chemical And Energy</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>b2c</t>
+          <t>B2C</t>
         </is>
       </c>
       <c r="J6" t="inlineStr"/>
@@ -2539,27 +2539,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>rrrworth sdn bhd</t>
+          <t>Rrrworth Sdn Bhd</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>lot f-1</t>
+          <t>Lot F-1</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> mpl saguking industrial estate. jalan</t>
+          <t xml:space="preserve"> Mpl Saguking Industrial Estate. Jalan</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>xx</t>
+          <t>Xx</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>selangor</t>
+          <t>Selangor</t>
         </is>
       </c>
       <c r="G7" t="n">
@@ -2568,7 +2568,7 @@
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr">
         <is>
-          <t>b2b</t>
+          <t>B2B</t>
         </is>
       </c>
       <c r="J7" t="inlineStr"/>
@@ -2581,27 +2581,27 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>cakeeeeee central sdn bhd</t>
+          <t>Cakeeeeee Central Sdn Bhd</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>36 jalan pju 1a/12,</t>
+          <t>36 Jalan Pju 1A/12,</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>taman perindustrian jaya</t>
+          <t>Taman Perindustrian Jaya</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>petaling jaya</t>
+          <t>Petaling Jaya</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>kuala lumpur</t>
+          <t>Kuala Lumpur</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -2619,7 +2619,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>tttt technologies sdn bhd</t>
+          <t>Tttt Technologies Sdn Bhd</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
@@ -2629,12 +2629,12 @@
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr">
         <is>
-          <t>manufacturing</t>
+          <t>Manufacturing</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>b2b</t>
+          <t>B2B</t>
         </is>
       </c>
       <c r="J9" t="inlineStr"/>
@@ -2647,27 +2647,27 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>uuuutech logistic</t>
+          <t>Uuuutech Logistic</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>lot 77, pt 5118, no.5 (ground floor),</t>
+          <t>Lot 77, Pt 5118, No.5 (Ground Floor),</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>jalan prima 5,</t>
+          <t>Jalan Prima 5,</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>port dickson</t>
+          <t>Port Dickson</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>melaka</t>
+          <t>Melaka</t>
         </is>
       </c>
       <c r="G10" t="n">
@@ -2685,23 +2685,23 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>zzzzzzfab industries sdn bhd</t>
+          <t>Zzzzzzfab Industries Sdn Bhd</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>29, jalan meru indah 20,</t>
+          <t>29, Jalan Meru Indah 20,</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
-          <t>klang</t>
+          <t>Klang</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>selangor</t>
+          <t>Selangor</t>
         </is>
       </c>
       <c r="G11" t="n">
@@ -2719,7 +2719,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>perfect company</t>
+          <t>Perfect Company</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
@@ -2780,7 +2780,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>uuuuu works sdn bhd</t>
+          <t>Uuuuu Works Sdn Bhd</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
@@ -2792,7 +2792,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ddd automotive</t>
+          <t>Ddd Automotive</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -2804,7 +2804,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>yyyyyy engineering and construction sdn bhd</t>
+          <t>Yyyyyy Engineering And Construction Sdn Bhd</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -2816,12 +2816,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>barber qqqqqqq sdn bhd</t>
+          <t>Barber Qqqqqqq Sdn Bhd</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>jnt</t>
+          <t>Jnt</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -2836,7 +2836,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>fgfgff-line sdn bhd</t>
+          <t>Fgfgff-Line Sdn Bhd</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -2852,7 +2852,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>rrrworth sdn bhd</t>
+          <t>Rrrworth Sdn Bhd</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
@@ -2864,7 +2864,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>cakeeeeee central sdn bhd</t>
+          <t>Cakeeeeee Central Sdn Bhd</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -2876,12 +2876,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>tttt technologies sdn bhd</t>
+          <t>Tttt Technologies Sdn Bhd</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>shopee express</t>
+          <t>Shopee Express</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -2896,7 +2896,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>uuuutech logistic</t>
+          <t>Uuuutech Logistic</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -2908,7 +2908,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>zzzzzzfab industries sdn bhd</t>
+          <t>Zzzzzzfab Industries Sdn Bhd</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
@@ -2920,7 +2920,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>perfect company</t>
+          <t>Perfect Company</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
@@ -2983,12 +2983,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>uuuuu works sdn bhd</t>
+          <t>Uuuuu Works Sdn Bhd</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>far</t>
+          <t>Far</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -2998,7 +2998,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>cleaner</t>
+          <t>Cleaner</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -3013,18 +3013,18 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ddd automotive</t>
+          <t>Ddd Automotive</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>zhong</t>
+          <t>Zhong</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>director</t>
+          <t>Director</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -3039,18 +3039,18 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>yyyyyy engineering and construction sdn bhd</t>
+          <t>Yyyyyy Engineering And Construction Sdn Bhd</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>wan</t>
+          <t>Wan</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>secretrary</t>
+          <t>Secretrary</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -3065,18 +3065,18 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>barber qqqqqqq sdn bhd</t>
+          <t>Barber Qqqqqqq Sdn Bhd</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ahmad</t>
+          <t>Ahmad</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
-          <t>executive</t>
+          <t>Executive</t>
         </is>
       </c>
       <c r="F5" t="inlineStr"/>
@@ -3087,12 +3087,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>fgfgff-line sdn bhd</t>
+          <t>Fgfgff-Line Sdn Bhd</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>kula</t>
+          <t>Kula</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -3102,7 +3102,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>technician</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -3117,12 +3117,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>rrrworth sdn bhd</t>
+          <t>Rrrworth Sdn Bhd</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>adam</t>
+          <t>Adam</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -3139,7 +3139,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>cakeeeeee central sdn bhd</t>
+          <t>Cakeeeeee Central Sdn Bhd</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -3153,7 +3153,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>tttt technologies sdn bhd</t>
+          <t>Tttt Technologies Sdn Bhd</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>uuuutech logistic</t>
+          <t>Uuuutech Logistic</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -3181,7 +3181,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>zzzzzzfab industries sdn bhd</t>
+          <t>Zzzzzzfab Industries Sdn Bhd</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
@@ -3195,7 +3195,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>perfect company</t>
+          <t>Perfect Company</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
@@ -3270,12 +3270,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>uuuuu works sdn bhd</t>
+          <t>Uuuuu Works Sdn Bhd</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>signup pages</t>
+          <t>Signup Pages</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
@@ -3298,12 +3298,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ddd automotive</t>
+          <t>Ddd Automotive</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>exhibition</t>
+          <t>Exhibition</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
@@ -3326,12 +3326,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>yyyyyy engineering and construction sdn bhd</t>
+          <t>Yyyyyy Engineering And Construction Sdn Bhd</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>twitter</t>
+          <t>Twitter</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
@@ -3354,12 +3354,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>barber qqqqqqq sdn bhd</t>
+          <t>Barber Qqqqqqq Sdn Bhd</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>signup pages</t>
+          <t>Signup Pages</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
@@ -3382,12 +3382,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>fgfgff-line sdn bhd</t>
+          <t>Fgfgff-Line Sdn Bhd</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>facebook</t>
+          <t>Facebook</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
@@ -3410,7 +3410,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>rrrworth sdn bhd</t>
+          <t>Rrrworth Sdn Bhd</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
@@ -3434,12 +3434,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>cakeeeeee central sdn bhd</t>
+          <t>Cakeeeeee Central Sdn Bhd</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>twitter</t>
+          <t>Twitter</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
@@ -3462,12 +3462,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>tttt technologies sdn bhd</t>
+          <t>Tttt Technologies Sdn Bhd</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>exhibition</t>
+          <t>Exhibition</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
@@ -3490,12 +3490,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>uuuutech logistic</t>
+          <t>Uuuutech Logistic</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>instagram</t>
+          <t>Instagram</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
@@ -3518,12 +3518,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>zzzzzzfab industries sdn bhd</t>
+          <t>Zzzzzzfab Industries Sdn Bhd</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>facebook</t>
+          <t>Facebook</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
@@ -3546,12 +3546,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>perfect company</t>
+          <t>Perfect Company</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>signup pages</t>
+          <t>Signup Pages</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -3615,7 +3615,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>uuuuu works sdn bhd</t>
+          <t>Uuuuu Works Sdn Bhd</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
@@ -3627,7 +3627,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ddd automotive</t>
+          <t>Ddd Automotive</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -3639,7 +3639,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>yyyyyy engineering and construction sdn bhd</t>
+          <t>Yyyyyy Engineering And Construction Sdn Bhd</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -3651,7 +3651,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>barber qqqqqqq sdn bhd</t>
+          <t>Barber Qqqqqqq Sdn Bhd</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
@@ -3663,7 +3663,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>fgfgff-line sdn bhd</t>
+          <t>Fgfgff-Line Sdn Bhd</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>rrrworth sdn bhd</t>
+          <t>Rrrworth Sdn Bhd</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
@@ -3687,7 +3687,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>cakeeeeee central sdn bhd</t>
+          <t>Cakeeeeee Central Sdn Bhd</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -3699,7 +3699,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>tttt technologies sdn bhd</t>
+          <t>Tttt Technologies Sdn Bhd</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
@@ -3711,7 +3711,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>uuuutech logistic</t>
+          <t>Uuuutech Logistic</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -3723,7 +3723,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>zzzzzzfab industries sdn bhd</t>
+          <t>Zzzzzzfab Industries Sdn Bhd</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
@@ -3735,7 +3735,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>perfect company</t>
+          <t>Perfect Company</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>

</xml_diff>